<commit_message>
Fix spreadsheet column names
</commit_message>
<xml_diff>
--- a/data/jimmy_butler_totals_playoffs.xlsx
+++ b/data/jimmy_butler_totals_playoffs.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
-    <t xml:space="preserve">By Year</t>
+    <t xml:space="preserve">YEAR</t>
   </si>
   <si>
     <t xml:space="preserve">TEAM </t>
@@ -161,6 +161,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,11 +183,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,20 +234,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,1051 +381,1051 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="1" width="7.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="4" t="n">
         <v>52.6</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="n">
+      <c r="J2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K2" s="3" t="n">
+      <c r="K2" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="M2" s="3" t="n">
+      <c r="M2" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="N2" s="4" t="n">
         <v>66.7</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="P2" s="3" t="n">
+      <c r="P2" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Q2" s="3" t="n">
+      <c r="Q2" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="R2" s="3" t="n">
+      <c r="R2" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="S2" s="3" t="n">
+      <c r="S2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T2" s="3" t="n">
+      <c r="T2" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="U2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3" t="n">
+      <c r="U2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="3" t="n">
+      <c r="W2" s="4" t="n">
         <v>56.4</v>
       </c>
-      <c r="X2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="3" t="n">
+      <c r="X2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="4" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>874</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>592</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>207</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="4" t="n">
         <v>442</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>46.8</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="4" t="n">
         <v>35.9</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="4" t="n">
         <v>186</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>80.6</v>
       </c>
-      <c r="O3" s="3" t="n">
+      <c r="O3" s="4" t="n">
         <v>47</v>
       </c>
-      <c r="P3" s="3" t="n">
+      <c r="P3" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="Q3" s="3" t="n">
+      <c r="Q3" s="4" t="n">
         <v>142</v>
       </c>
-      <c r="R3" s="3" t="n">
+      <c r="R3" s="4" t="n">
         <v>129</v>
       </c>
-      <c r="S3" s="3" t="n">
+      <c r="S3" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="T3" s="3" t="n">
+      <c r="T3" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U3" s="3" t="n">
+      <c r="U3" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="V3" s="3" t="n">
+      <c r="V3" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W3" s="3" t="n">
+      <c r="W3" s="4" t="n">
         <v>1076.9</v>
       </c>
-      <c r="X3" s="3" t="n">
+      <c r="X3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Y3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="3" t="n">
+      <c r="Y3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="4" t="n">
         <v>-11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>629</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>466</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>166</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="4" t="n">
         <v>328</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>50.6</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <v>68</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="4" t="n">
         <v>33.8</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <v>111</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <v>132</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="4" t="n">
         <v>84.1</v>
       </c>
-      <c r="O4" s="3" t="n">
+      <c r="O4" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="P4" s="3" t="n">
+      <c r="P4" s="4" t="n">
         <v>84</v>
       </c>
-      <c r="Q4" s="3" t="n">
+      <c r="Q4" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="R4" s="3" t="n">
+      <c r="R4" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="S4" s="3" t="n">
+      <c r="S4" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="T4" s="3" t="n">
+      <c r="T4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U4" s="3" t="n">
+      <c r="U4" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="V4" s="3" t="n">
+      <c r="V4" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="W4" s="3" t="n">
+      <c r="W4" s="4" t="n">
         <v>846</v>
       </c>
-      <c r="X4" s="3" t="n">
+      <c r="X4" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Y4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="3" t="n">
+      <c r="Y4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="4" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>154</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>58</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="4" t="n">
         <v>64</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="4" t="n">
         <v>29.7</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="4" t="n">
         <v>26.7</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="4" t="n">
         <v>72.7</v>
       </c>
-      <c r="O5" s="3" t="n">
+      <c r="O5" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="P5" s="3" t="n">
+      <c r="P5" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="Q5" s="3" t="n">
+      <c r="Q5" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="R5" s="3" t="n">
+      <c r="R5" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="S5" s="3" t="n">
+      <c r="S5" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="T5" s="3" t="n">
+      <c r="T5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="U5" s="3" t="n">
+      <c r="U5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="V5" s="3" t="n">
+      <c r="V5" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="W5" s="3" t="n">
+      <c r="W5" s="4" t="n">
         <v>145</v>
       </c>
-      <c r="X5" s="3" t="n">
+      <c r="X5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="Y5" s="3" t="n">
+      <c r="Y5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" s="3" t="n">
+      <c r="Z5" s="4" t="n">
         <v>-86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>806</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>467</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>144</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <v>295</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>48.8</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="4" t="n">
         <v>34.9</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <v>164</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <v>191</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="4" t="n">
         <v>85.9</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="O6" s="4" t="n">
         <v>46</v>
       </c>
-      <c r="P6" s="3" t="n">
+      <c r="P6" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="Q6" s="3" t="n">
+      <c r="Q6" s="4" t="n">
         <v>136</v>
       </c>
-      <c r="R6" s="3" t="n">
+      <c r="R6" s="4" t="n">
         <v>127</v>
       </c>
-      <c r="S6" s="3" t="n">
+      <c r="S6" s="4" t="n">
         <v>59</v>
       </c>
-      <c r="T6" s="3" t="n">
+      <c r="T6" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="U6" s="3" t="n">
+      <c r="U6" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="V6" s="3" t="n">
+      <c r="V6" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W6" s="3" t="n">
+      <c r="W6" s="4" t="n">
         <v>926.7</v>
       </c>
-      <c r="X6" s="3" t="n">
+      <c r="X6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Y6" s="3" t="n">
+      <c r="Y6" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="Z6" s="3" t="n">
+      <c r="Z6" s="4" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>421</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>233</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>79</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="4" t="n">
         <v>175</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>45.1</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="4" t="n">
         <v>26.7</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="4" t="n">
         <v>63</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="4" t="n">
         <v>72</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="N7" s="4" t="n">
         <v>87.5</v>
       </c>
-      <c r="O7" s="3" t="n">
+      <c r="O7" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="P7" s="3" t="n">
+      <c r="P7" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="Q7" s="3" t="n">
+      <c r="Q7" s="4" t="n">
         <v>72</v>
       </c>
-      <c r="R7" s="3" t="n">
+      <c r="R7" s="4" t="n">
         <v>62</v>
       </c>
-      <c r="S7" s="3" t="n">
+      <c r="S7" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="T7" s="3" t="n">
+      <c r="T7" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="U7" s="3" t="n">
+      <c r="U7" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="V7" s="3" t="n">
+      <c r="V7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W7" s="3" t="n">
+      <c r="W7" s="4" t="n">
         <v>465.4</v>
       </c>
-      <c r="X7" s="3" t="n">
+      <c r="X7" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="Y7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="3" t="n">
+      <c r="Y7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="4" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>170</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>79</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="G8" s="3" t="n">
+      <c r="G8" s="4" t="n">
         <v>63</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="4" t="n">
         <v>44.4</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="K8" s="4" t="n">
         <v>47.1</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="N8" s="4" t="n">
         <v>83.3</v>
       </c>
-      <c r="O8" s="3" t="n">
+      <c r="O8" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="P8" s="3" t="n">
+      <c r="P8" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="Q8" s="3" t="n">
+      <c r="Q8" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="R8" s="3" t="n">
+      <c r="R8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S8" s="3" t="n">
+      <c r="S8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="T8" s="3" t="n">
+      <c r="T8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="U8" s="3" t="n">
+      <c r="U8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="V8" s="3" t="n">
+      <c r="V8" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="W8" s="3" t="n">
+      <c r="W8" s="4" t="n">
         <v>155</v>
       </c>
-      <c r="X8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3" t="n">
+      <c r="X8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4" t="n">
         <v>-12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>239</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>136</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <v>46</v>
       </c>
-      <c r="G9" s="3" t="n">
+      <c r="G9" s="4" t="n">
         <v>108</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="4" t="n">
         <v>42.6</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K9" s="3" t="n">
+      <c r="K9" s="4" t="n">
         <v>26.1</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="4" t="n">
         <v>47</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="4" t="n">
         <v>80.9</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="O9" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="P9" s="3" t="n">
+      <c r="P9" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q9" s="3" t="n">
+      <c r="Q9" s="4" t="n">
         <v>44</v>
       </c>
-      <c r="R9" s="3" t="n">
+      <c r="R9" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="S9" s="3" t="n">
+      <c r="S9" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="T9" s="3" t="n">
+      <c r="T9" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="U9" s="3" t="n">
+      <c r="U9" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="V9" s="3" t="n">
+      <c r="V9" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="W9" s="3" t="n">
+      <c r="W9" s="4" t="n">
         <v>257.8</v>
       </c>
-      <c r="X9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="3" t="n">
+      <c r="X9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="4" t="n">
         <v>-42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>506</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>275</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>94</v>
       </c>
-      <c r="G10" s="3" t="n">
+      <c r="G10" s="4" t="n">
         <v>213</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <v>44.1</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="4" t="n">
         <v>72</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="4" t="n">
         <v>38.9</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="4" t="n">
         <v>59</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="4" t="n">
         <v>72</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="N10" s="4" t="n">
         <v>81.9</v>
       </c>
-      <c r="O10" s="3" t="n">
+      <c r="O10" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="P10" s="3" t="n">
+      <c r="P10" s="4" t="n">
         <v>49</v>
       </c>
-      <c r="Q10" s="3" t="n">
+      <c r="Q10" s="4" t="n">
         <v>67</v>
       </c>
-      <c r="R10" s="3" t="n">
+      <c r="R10" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="S10" s="3" t="n">
+      <c r="S10" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="T10" s="3" t="n">
+      <c r="T10" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="U10" s="3" t="n">
+      <c r="U10" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="V10" s="3" t="n">
+      <c r="V10" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="W10" s="3" t="n">
+      <c r="W10" s="4" t="n">
         <v>505.4</v>
       </c>
-      <c r="X10" s="3" t="n">
+      <c r="X10" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Y10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="3" t="n">
+      <c r="Y10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="4" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>218</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <v>68</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="4" t="n">
         <v>57</v>
       </c>
-      <c r="H11" s="3" t="n">
+      <c r="H11" s="4" t="n">
         <v>38.6</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="J11" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="K11" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="N11" s="4" t="n">
         <v>78.3</v>
       </c>
-      <c r="O11" s="3" t="n">
+      <c r="O11" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="P11" s="3" t="n">
+      <c r="P11" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q11" s="3" t="n">
+      <c r="Q11" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="R11" s="3" t="n">
+      <c r="R11" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="S11" s="3" t="n">
+      <c r="S11" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="T11" s="3" t="n">
+      <c r="T11" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="U11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" s="3" t="n">
+      <c r="U11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="W11" s="3" t="n">
+      <c r="W11" s="4" t="n">
         <v>130.7</v>
       </c>
-      <c r="X11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="3" t="n">
+      <c r="X11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="4" t="n">
         <v>-23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>490</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="4" t="n">
         <v>160</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="4" t="n">
         <v>115</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="4" t="n">
         <v>43.5</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="J12" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="K12" s="4" t="n">
         <v>40.5</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="N12" s="4" t="n">
         <v>81.8</v>
       </c>
-      <c r="O12" s="3" t="n">
+      <c r="O12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="P12" s="3" t="n">
+      <c r="P12" s="4" t="n">
         <v>53</v>
       </c>
-      <c r="Q12" s="3" t="n">
+      <c r="Q12" s="4" t="n">
         <v>62</v>
       </c>
-      <c r="R12" s="3" t="n">
+      <c r="R12" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S12" s="3" t="n">
+      <c r="S12" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="T12" s="3" t="n">
+      <c r="T12" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="U12" s="3" t="n">
+      <c r="U12" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="V12" s="3" t="n">
+      <c r="V12" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="W12" s="3" t="n">
+      <c r="W12" s="4" t="n">
         <v>329.4</v>
       </c>
-      <c r="X12" s="3" t="n">
+      <c r="X12" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Y12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="3" t="n">
+      <c r="Y12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4" t="n">
         <v>-93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" s="3" t="n">
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="W13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="3" t="n">
+      <c r="W13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="4" t="n">
         <v>-7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Jimmy playoff totals speadsheet
</commit_message>
<xml_diff>
--- a/data/jimmy_butler_totals_playoffs.xlsx
+++ b/data/jimmy_butler_totals_playoffs.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="X15" activeCellId="0" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,76 +477,76 @@
         <v>27</v>
       </c>
       <c r="C2" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>320</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>180</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>59</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>132</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="N2" s="4" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="O2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="R2" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="S2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="T2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="U2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="W2" s="4" t="n">
+        <v>354.2</v>
+      </c>
+      <c r="X2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>42</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="M2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="N2" s="4" t="n">
-        <v>66.7</v>
-      </c>
-      <c r="O2" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="P2" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="R2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="S2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="U2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="W2" s="4" t="n">
-        <v>56.4</v>
-      </c>
-      <c r="X2" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="Y2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="Z2" s="4" t="n">
-        <v>14</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update Jimmy playoff totals spreadsheet
</commit_message>
<xml_diff>
--- a/data/jimmy_butler_totals_playoffs.xlsx
+++ b/data/jimmy_butler_totals_playoffs.xlsx
@@ -234,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,6 +249,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -381,7 +385,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X15" activeCellId="0" sqref="X15"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,23 +477,23 @@
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>320</v>
+        <v>397</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>44.7</v>
@@ -498,46 +502,46 @@
         <v>11</v>
       </c>
       <c r="J2" s="4" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K2" s="4" t="n">
-        <v>34.4</v>
+        <v>30.6</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="M2" s="4" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="N2" s="4" t="n">
-        <v>79.7</v>
+        <v>80</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="P2" s="4" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="R2" s="4" t="n">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="S2" s="4" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="T2" s="4" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="U2" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V2" s="4" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="W2" s="4" t="n">
-        <v>354.2</v>
+        <v>422.1</v>
       </c>
       <c r="X2" s="4" t="n">
         <v>1</v>
@@ -546,886 +550,886 @@
         <v>0</v>
       </c>
       <c r="Z2" s="4" t="n">
-        <v>-6</v>
+        <v>-53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>874</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="5" t="n">
         <v>592</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="5" t="n">
         <v>207</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <v>442</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="5" t="n">
         <v>46.8</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="5" t="n">
         <v>78</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="5" t="n">
         <v>35.9</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="M3" s="5" t="n">
         <v>186</v>
       </c>
-      <c r="N3" s="4" t="n">
+      <c r="N3" s="5" t="n">
         <v>80.6</v>
       </c>
-      <c r="O3" s="4" t="n">
+      <c r="O3" s="5" t="n">
         <v>47</v>
       </c>
-      <c r="P3" s="4" t="n">
+      <c r="P3" s="5" t="n">
         <v>95</v>
       </c>
-      <c r="Q3" s="4" t="n">
+      <c r="Q3" s="5" t="n">
         <v>142</v>
       </c>
-      <c r="R3" s="4" t="n">
+      <c r="R3" s="5" t="n">
         <v>129</v>
       </c>
-      <c r="S3" s="4" t="n">
+      <c r="S3" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="T3" s="4" t="n">
+      <c r="T3" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="U3" s="4" t="n">
+      <c r="U3" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="V3" s="4" t="n">
+      <c r="V3" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="W3" s="4" t="n">
+      <c r="W3" s="5" t="n">
         <v>1076.9</v>
       </c>
-      <c r="X3" s="4" t="n">
+      <c r="X3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Y3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="4" t="n">
+      <c r="Y3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5" t="n">
         <v>-11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>629</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="5" t="n">
         <v>466</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>166</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <v>328</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="5" t="n">
         <v>50.6</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="5" t="n">
         <v>68</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="5" t="n">
         <v>33.8</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="5" t="n">
         <v>111</v>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="M4" s="5" t="n">
         <v>132</v>
       </c>
-      <c r="N4" s="4" t="n">
+      <c r="N4" s="5" t="n">
         <v>84.1</v>
       </c>
-      <c r="O4" s="4" t="n">
+      <c r="O4" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="P4" s="4" t="n">
+      <c r="P4" s="5" t="n">
         <v>84</v>
       </c>
-      <c r="Q4" s="4" t="n">
+      <c r="Q4" s="5" t="n">
         <v>125</v>
       </c>
-      <c r="R4" s="4" t="n">
+      <c r="R4" s="5" t="n">
         <v>78</v>
       </c>
-      <c r="S4" s="4" t="n">
+      <c r="S4" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="T4" s="4" t="n">
+      <c r="T4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="U4" s="4" t="n">
+      <c r="U4" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="V4" s="4" t="n">
+      <c r="V4" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="W4" s="4" t="n">
+      <c r="W4" s="5" t="n">
         <v>846</v>
       </c>
-      <c r="X4" s="4" t="n">
+      <c r="X4" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Y4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="4" t="n">
+      <c r="Y4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>154</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>58</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="5" t="n">
         <v>64</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="5" t="n">
         <v>29.7</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="5" t="n">
         <v>26.7</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="N5" s="4" t="n">
+      <c r="N5" s="5" t="n">
         <v>72.7</v>
       </c>
-      <c r="O5" s="4" t="n">
+      <c r="O5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="P5" s="4" t="n">
+      <c r="P5" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="Q5" s="4" t="n">
+      <c r="Q5" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="R5" s="4" t="n">
+      <c r="R5" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="S5" s="4" t="n">
+      <c r="S5" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="T5" s="4" t="n">
+      <c r="T5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="U5" s="4" t="n">
+      <c r="U5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="V5" s="4" t="n">
+      <c r="V5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="W5" s="4" t="n">
+      <c r="W5" s="5" t="n">
         <v>145</v>
       </c>
-      <c r="X5" s="4" t="n">
+      <c r="X5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="Y5" s="4" t="n">
+      <c r="Y5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" s="4" t="n">
+      <c r="Z5" s="5" t="n">
         <v>-86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="5" t="n">
         <v>806</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <v>467</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="5" t="n">
         <v>144</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="5" t="n">
         <v>295</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="5" t="n">
         <v>48.8</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="5" t="n">
         <v>43</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="5" t="n">
         <v>34.9</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="5" t="n">
         <v>164</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="5" t="n">
         <v>191</v>
       </c>
-      <c r="N6" s="4" t="n">
+      <c r="N6" s="5" t="n">
         <v>85.9</v>
       </c>
-      <c r="O6" s="4" t="n">
+      <c r="O6" s="5" t="n">
         <v>46</v>
       </c>
-      <c r="P6" s="4" t="n">
+      <c r="P6" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="Q6" s="4" t="n">
+      <c r="Q6" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="R6" s="4" t="n">
+      <c r="R6" s="5" t="n">
         <v>127</v>
       </c>
-      <c r="S6" s="4" t="n">
+      <c r="S6" s="5" t="n">
         <v>59</v>
       </c>
-      <c r="T6" s="4" t="n">
+      <c r="T6" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="U6" s="4" t="n">
+      <c r="U6" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="V6" s="4" t="n">
+      <c r="V6" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="W6" s="4" t="n">
+      <c r="W6" s="5" t="n">
         <v>926.7</v>
       </c>
-      <c r="X6" s="4" t="n">
+      <c r="X6" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Y6" s="4" t="n">
+      <c r="Y6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="Z6" s="4" t="n">
+      <c r="Z6" s="5" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
         <v>421</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="5" t="n">
         <v>233</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>79</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="5" t="n">
         <v>175</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="5" t="n">
         <v>45.1</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="5" t="n">
         <v>26.7</v>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="M7" s="4" t="n">
+      <c r="M7" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="N7" s="4" t="n">
+      <c r="N7" s="5" t="n">
         <v>87.5</v>
       </c>
-      <c r="O7" s="4" t="n">
+      <c r="O7" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="P7" s="4" t="n">
+      <c r="P7" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="Q7" s="4" t="n">
+      <c r="Q7" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="R7" s="4" t="n">
+      <c r="R7" s="5" t="n">
         <v>62</v>
       </c>
-      <c r="S7" s="4" t="n">
+      <c r="S7" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="T7" s="4" t="n">
+      <c r="T7" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="U7" s="4" t="n">
+      <c r="U7" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="V7" s="4" t="n">
+      <c r="V7" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="W7" s="4" t="n">
+      <c r="W7" s="5" t="n">
         <v>465.4</v>
       </c>
-      <c r="X7" s="4" t="n">
+      <c r="X7" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="Y7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="4" t="n">
+      <c r="Y7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="5" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>170</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <v>79</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="5" t="n">
         <v>44.4</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="5" t="n">
         <v>47.1</v>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L8" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="M8" s="4" t="n">
+      <c r="M8" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="N8" s="4" t="n">
+      <c r="N8" s="5" t="n">
         <v>83.3</v>
       </c>
-      <c r="O8" s="4" t="n">
+      <c r="O8" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="P8" s="4" t="n">
+      <c r="P8" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="Q8" s="4" t="n">
+      <c r="Q8" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="R8" s="4" t="n">
+      <c r="R8" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="S8" s="4" t="n">
+      <c r="S8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="T8" s="4" t="n">
+      <c r="T8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="U8" s="4" t="n">
+      <c r="U8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="V8" s="4" t="n">
+      <c r="V8" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="W8" s="4" t="n">
+      <c r="W8" s="5" t="n">
         <v>155</v>
       </c>
-      <c r="X8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="4" t="n">
+      <c r="X8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="5" t="n">
         <v>-12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="5" t="n">
         <v>239</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>46</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="5" t="n">
         <v>108</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="5" t="n">
         <v>42.6</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="I9" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K9" s="5" t="n">
         <v>26.1</v>
       </c>
-      <c r="L9" s="4" t="n">
+      <c r="L9" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="M9" s="4" t="n">
+      <c r="M9" s="5" t="n">
         <v>47</v>
       </c>
-      <c r="N9" s="4" t="n">
+      <c r="N9" s="5" t="n">
         <v>80.9</v>
       </c>
-      <c r="O9" s="4" t="n">
+      <c r="O9" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="P9" s="4" t="n">
+      <c r="P9" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q9" s="4" t="n">
+      <c r="Q9" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="R9" s="4" t="n">
+      <c r="R9" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="S9" s="4" t="n">
+      <c r="S9" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="T9" s="4" t="n">
+      <c r="T9" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="U9" s="4" t="n">
+      <c r="U9" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="V9" s="4" t="n">
+      <c r="V9" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="W9" s="4" t="n">
+      <c r="W9" s="5" t="n">
         <v>257.8</v>
       </c>
-      <c r="X9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="4" t="n">
+      <c r="X9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="5" t="n">
         <v>-42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="5" t="n">
         <v>506</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="5" t="n">
         <v>275</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>94</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="5" t="n">
         <v>213</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="5" t="n">
         <v>44.1</v>
       </c>
-      <c r="I10" s="4" t="n">
+      <c r="I10" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="K10" s="4" t="n">
+      <c r="K10" s="5" t="n">
         <v>38.9</v>
       </c>
-      <c r="L10" s="4" t="n">
+      <c r="L10" s="5" t="n">
         <v>59</v>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="M10" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="N10" s="4" t="n">
+      <c r="N10" s="5" t="n">
         <v>81.9</v>
       </c>
-      <c r="O10" s="4" t="n">
+      <c r="O10" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="P10" s="4" t="n">
+      <c r="P10" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="Q10" s="4" t="n">
+      <c r="Q10" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="R10" s="4" t="n">
+      <c r="R10" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="S10" s="4" t="n">
+      <c r="S10" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="T10" s="4" t="n">
+      <c r="T10" s="5" t="n">
         <v>29</v>
       </c>
-      <c r="U10" s="4" t="n">
+      <c r="U10" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="V10" s="4" t="n">
+      <c r="V10" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="W10" s="4" t="n">
+      <c r="W10" s="5" t="n">
         <v>505.4</v>
       </c>
-      <c r="X10" s="4" t="n">
+      <c r="X10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="4" t="n">
+      <c r="Y10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="5" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>218</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="5" t="n">
         <v>68</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="5" t="n">
         <v>57</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="5" t="n">
         <v>38.6</v>
       </c>
-      <c r="I11" s="4" t="n">
+      <c r="I11" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="K11" s="4" t="n">
+      <c r="K11" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="L11" s="4" t="n">
+      <c r="L11" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="M11" s="4" t="n">
+      <c r="M11" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="N11" s="4" t="n">
+      <c r="N11" s="5" t="n">
         <v>78.3</v>
       </c>
-      <c r="O11" s="4" t="n">
+      <c r="O11" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="P11" s="4" t="n">
+      <c r="P11" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="Q11" s="4" t="n">
+      <c r="Q11" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="R11" s="4" t="n">
+      <c r="R11" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S11" s="4" t="n">
+      <c r="S11" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="T11" s="4" t="n">
+      <c r="T11" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="U11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" s="4" t="n">
+      <c r="U11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="W11" s="4" t="n">
+      <c r="W11" s="5" t="n">
         <v>130.7</v>
       </c>
-      <c r="X11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="4" t="n">
+      <c r="X11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="5" t="n">
         <v>-23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>490</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="5" t="n">
         <v>160</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="5" t="n">
         <v>115</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="5" t="n">
         <v>43.5</v>
       </c>
-      <c r="I12" s="4" t="n">
+      <c r="I12" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="K12" s="4" t="n">
+      <c r="K12" s="5" t="n">
         <v>40.5</v>
       </c>
-      <c r="L12" s="4" t="n">
+      <c r="L12" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="M12" s="4" t="n">
+      <c r="M12" s="5" t="n">
         <v>55</v>
       </c>
-      <c r="N12" s="4" t="n">
+      <c r="N12" s="5" t="n">
         <v>81.8</v>
       </c>
-      <c r="O12" s="4" t="n">
+      <c r="O12" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="P12" s="4" t="n">
+      <c r="P12" s="5" t="n">
         <v>53</v>
       </c>
-      <c r="Q12" s="4" t="n">
+      <c r="Q12" s="5" t="n">
         <v>62</v>
       </c>
-      <c r="R12" s="4" t="n">
+      <c r="R12" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="S12" s="4" t="n">
+      <c r="S12" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="T12" s="4" t="n">
+      <c r="T12" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="U12" s="4" t="n">
+      <c r="U12" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="V12" s="4" t="n">
+      <c r="V12" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="W12" s="4" t="n">
+      <c r="W12" s="5" t="n">
         <v>329.4</v>
       </c>
-      <c r="X12" s="4" t="n">
+      <c r="X12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="4" t="n">
+      <c r="Y12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="5" t="n">
         <v>-93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" s="4" t="n">
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="W13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="4" t="n">
+      <c r="W13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="5" t="n">
         <v>-7</v>
       </c>
     </row>

</xml_diff>